<commit_message>
updated class OpenRandomCell. Delete Extensions
</commit_message>
<xml_diff>
--- a/MySudokuGame/Rating/Rating.xlsx
+++ b/MySudokuGame/Rating/Rating.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Easy</t>
   </si>
@@ -46,6 +46,36 @@
   </si>
   <si>
     <t>00:13:18</t>
+  </si>
+  <si>
+    <t>00:17:60</t>
+  </si>
+  <si>
+    <t>00:44:94</t>
+  </si>
+  <si>
+    <t>00:07:54</t>
+  </si>
+  <si>
+    <t>03:32:84</t>
+  </si>
+  <si>
+    <t>01:14:28</t>
+  </si>
+  <si>
+    <t>01:30:01</t>
+  </si>
+  <si>
+    <t>00:05:39</t>
+  </si>
+  <si>
+    <t>00:06:16</t>
+  </si>
+  <si>
+    <t>00:34:93</t>
+  </si>
+  <si>
+    <t>01:06:20</t>
   </si>
 </sst>
 </file>
@@ -372,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A1:C5"/>
@@ -419,6 +449,56 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>